<commit_message>
array de teste no lab
</commit_message>
<xml_diff>
--- a/sensor_data.xlsx
+++ b/sensor_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\P&amp;D\Grade-SAE\Sistema supervisório\teste_grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1C9E3-A6DB-4A89-9806-C7F8FDAABF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77BD813-6090-4ADF-9CC3-D83D1D198928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{FBBB33E6-0A39-4BD0-872A-A59064315D15}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{FBBB33E6-0A39-4BD0-872A-A59064315D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Grade" sheetId="1" r:id="rId1"/>
     <sheet name="Demonstração" sheetId="2" r:id="rId2"/>
+    <sheet name="Validação" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>Sensor</t>
   </si>
@@ -91,13 +92,19 @@
   </si>
   <si>
     <t>169-35</t>
+  </si>
+  <si>
+    <t>250-50</t>
+  </si>
+  <si>
+    <t>168-45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +122,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -159,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,14 +496,14 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="5" max="11" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="5" max="11" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +540,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -552,7 +569,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -583,7 +600,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -614,10 +631,10 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M8" s="7"/>
     </row>
   </sheetData>
@@ -630,18 +647,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2A8DB3-4ECF-4019-AD60-8B41F9D69E15}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
     <col min="5" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +695,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -709,7 +726,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -742,4 +759,119 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2F9F52-B70C-41AA-8F50-F8C81C569C06}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1550.4313083333336</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="I2" s="5">
+        <v>7.3</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>20.409904278669277</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1545.2719999999999</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5">
+        <v>34.6</v>
+      </c>
+      <c r="G3" s="5">
+        <v>-0.7</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>